<commit_message>
update file test case
</commit_message>
<xml_diff>
--- a/Budget_request_Testcase.xlsx
+++ b/Budget_request_Testcase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebdriverIO\ProjectTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BE4CEE2-89D5-49D1-BCA1-F7CECA7875FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1882AD-14FC-4EA6-9AAE-1F811BA2BC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{432D4B3D-68B6-4C3C-8E61-5866CAD55930}"/>
   </bookViews>
@@ -63,76 +63,11 @@
     <t>STT</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. Verify documment is add
-2.1 Request display in page request and reject status
-2.2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Button Send accountant display</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> in page detail 
-3.1 Approve success and approved status
-3.2 Login For Board of directors account and verify request not display 
-3.3 Login For Financial Admin account and verify request display
-4.1 Status change success 
-4.2  Login Head of department account and verify notification display 
-4.3  Login Accountant account account and verify notification display</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">1. Add documnent for request
 2. Click send accountant
 3. Login Accountant account and approve for request
 4. Login Board of directors account and approve for request
 </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. Verify documment is add
-2.  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Button Send accountant display</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and Request display in page request and approve status
-3.1 Approve success and approved status
-3.2  Login For Financial Admin account and verify request not display 
-3.3 Login For Board of directors account and verify request display 
-4.1 Status change success 
-4.2  Login Head of department account and verify notification display 
-4.3  Login Accountant account account and verify notification display</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">1. Add documnent for request
@@ -153,24 +88,6 @@
     <t xml:space="preserve">1. Login Head of department account and approve for request 
 2. Login Accountant account and approve for request 
 3. Login For Board of directors account and approve for request </t>
-  </si>
-  <si>
-    <t>1. Verify request approve by Head of department
-2.1 Verify request approve by Accountant account
-2.2 Status change success 
-2.3 Login For Board of directors account and verify request not display 
-2.4 Login For Financial Admin account and verify request display
-3.1  Login Head of department account and verify notification display 
-3.2  Login Accountant account account and verify notification display</t>
-  </si>
-  <si>
-    <t>1. Verify request approve by Head of department
-2.1 Verify request approve by Accountant account
-2.2 Status change success 
-2.3 Login Financial Admin account and verify request not display 
-3.3 Login Board of directors account and verify request display
-3.1  Login Head of department account and verify notification display 
-3.2  Login Accountant account account and verify notification display</t>
   </si>
   <si>
     <t xml:space="preserve">1. Login Head of department account and approve for request 
@@ -387,36 +304,6 @@
 2. Finance invalid value</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. Request subject  valid
-2. Request number finance is not empty
-3. Document  valid 
-4. Request display in page request
-5. Change Head of department reject status and verify reason reject.
-6. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Button Send accountant not display </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>and Button send Head of department display</t>
-    </r>
-  </si>
-  <si>
     <t>[documnent final] = "bill_final.exe"</t>
   </si>
   <si>
@@ -485,6 +372,191 @@
 5.2   Login accountant account  and Verify notification send request success </t>
   </si>
   <si>
+    <t>Precondition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID Test Case </t>
+  </si>
+  <si>
+    <t>ID Test Suite</t>
+  </si>
+  <si>
+    <r>
+      <t>1. Request subject  valid
+2. Request number finance valid
+3. Document  valid 
+4. Request display in page request and approve status
+5. Approve success and change Head of department approved status
+6. Verify</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> reason reject and status </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Request subject  valid
+2. Request number finance valid
+3. Document  valid 
+4. Request display in page request
+5. Change Head of department reject status and verify reason reject.
+6. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Button Send accountant not display </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and Button send Head of department display</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Verify documment is add
+2.  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Button Send accountant display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and Request display in page request and wait for approve status
+3.1 Approve success and approved status
+3.2 Login For Board of directors account and verify request not display 
+3.3 Login For Financial Admin account and verify request display
+4.1 Status change success 
+4.2  Login Head of department account and verify notification display 
+4.3  Login Accountant account account and verify notification display</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Verify documment is add
+2.  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Button Send accountant display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and Request display in page request and wait for approve status
+3.1 Approve success and approved status
+3.2  Login For Financial Admin account and verify request not display 
+3.3 Login For Board of directors account and verify request display 
+4.1 Status change success 
+4.2  Login Head of department account and verify notification display 
+4.3  Login Accountant account account and verify notification display</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Verify request approve by Head of department
+2.1 Verify request approve by Accountant account
+2.2 Status change success 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2.3 Login For Board of directors account and verify request not display 
+2.4 Login For Financial Admin account and verify request display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3.1  Login Head of department account and verify notification display 
+3.2  Login Accountant account account and verify notification display</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Verify request approve by Head of department
+2.1 Verify request approve by Accountant account
+2.2 Status change success 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2.3 Login Financial Admin account and verify request not display 
+2.4 Login Board of directors account and verify request display
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3.1  Login Head of department account and verify notification display 
+3.2  Login Accountant account account and verify notification display</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">1. Request subject  valid
 2. Request number finance valid
@@ -501,7 +573,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Accountant account</t>
+      <t>accountant account</t>
     </r>
     <r>
       <rPr>
@@ -513,35 +585,6 @@
       </rPr>
       <t xml:space="preserve"> approved status
 </t>
-    </r>
-  </si>
-  <si>
-    <t>Precondition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID Test Case </t>
-  </si>
-  <si>
-    <t>ID Test Suite</t>
-  </si>
-  <si>
-    <r>
-      <t>1. Request subject  valid
-2. Request number finance valid
-3. Document  valid 
-4. Request display in page request and approve status
-5. Approve success and change Head of department approved status
-6. Verify</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> reason reject and status </t>
     </r>
   </si>
 </sst>
@@ -659,10 +702,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -684,10 +727,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -990,7 +1029,7 @@
   <dimension ref="A4:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,19 +1050,19 @@
         <v>7</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>1</v>
@@ -1039,7 +1078,7 @@
       <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1049,13 +1088,13 @@
         <v>5</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -1064,21 +1103,21 @@
       <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="7"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -1087,21 +1126,21 @@
       <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="7"/>
+      <c r="B7" s="8"/>
       <c r="C7" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -1110,21 +1149,21 @@
       <c r="A8" s="2">
         <v>4</v>
       </c>
-      <c r="B8" s="7"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -1133,21 +1172,21 @@
       <c r="A9" s="2">
         <v>5</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -1156,21 +1195,21 @@
       <c r="A10" s="2">
         <v>6</v>
       </c>
-      <c r="B10" s="7"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -1179,21 +1218,21 @@
       <c r="A11" s="2">
         <v>7</v>
       </c>
-      <c r="B11" s="7"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -1202,21 +1241,21 @@
       <c r="A12" s="2">
         <v>8</v>
       </c>
-      <c r="B12" s="7"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -1225,21 +1264,21 @@
       <c r="A13" s="2">
         <v>9</v>
       </c>
-      <c r="B13" s="7"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -1248,21 +1287,21 @@
       <c r="A14" s="2">
         <v>10</v>
       </c>
-      <c r="B14" s="7"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -1273,72 +1312,72 @@
         <v>11</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="225" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>12</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>13</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -1348,22 +1387,22 @@
         <v>14</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="F18" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -1373,29 +1412,29 @@
         <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="8"/>
+      <c r="B20" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I4" xr:uid="{13AE7274-7AB8-410B-9563-8384048EE252}"/>

</xml_diff>